<commit_message>
train on new labels
</commit_message>
<xml_diff>
--- a/Resources/ROI_CT.xlsx
+++ b/Resources/ROI_CT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/achs/Library/Mobile Documents/com~apple~CloudDocs/Australia/PhD/Resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/achs/PhD/code/CT-MRI_LandmarkDetection/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB1F161-02A1-6B48-875E-15D2518A193E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E76950-8CD0-E141-ABA9-5D68687BF5D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -182,9 +185,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -468,31 +470,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="169" workbookViewId="0">
+      <selection activeCell="N56" sqref="N56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
       <c r="F1" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
       <c r="O1" t="s">
         <v>31</v>
       </c>
@@ -504,13 +502,13 @@
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>26</v>
       </c>
       <c r="F2" t="s">
@@ -522,22 +520,22 @@
       <c r="H2" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="1" t="s">
         <v>26</v>
       </c>
       <c r="O2" t="s">
@@ -575,13 +573,13 @@
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>758</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3">
         <v>449</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3">
         <v>207</v>
       </c>
       <c r="F3">
@@ -593,24 +591,24 @@
       <c r="H3">
         <v>207</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3">
         <v>757</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3">
         <v>448</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3">
         <v>207</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="1">
         <f>MEDIAN(C3,F3,I3)</f>
         <v>758</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="1">
         <f>MEDIAN(D3,G3,J3)</f>
         <v>449</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3" s="1">
         <f>MEDIAN(E3,H3,K3)</f>
         <v>207</v>
       </c>
@@ -658,13 +656,13 @@
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>751</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4">
         <v>478</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4">
         <v>205</v>
       </c>
       <c r="F4">
@@ -676,24 +674,24 @@
       <c r="H4">
         <v>205</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4">
         <v>751</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4">
         <v>479</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4">
         <v>207</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="1">
         <f t="shared" ref="L4:L67" si="3">MEDIAN(C4,F4,I4)</f>
         <v>751</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="1">
         <f t="shared" ref="M4:M67" si="4">MEDIAN(D4,G4,J4)</f>
         <v>478</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="1">
         <f t="shared" ref="N4:N67" si="5">MEDIAN(E4,H4,K4)</f>
         <v>205</v>
       </c>
@@ -741,13 +739,13 @@
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
         <v>243</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
         <v>475</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5">
         <v>214</v>
       </c>
       <c r="F5">
@@ -759,24 +757,24 @@
       <c r="H5">
         <v>214</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5">
         <v>243</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5">
         <v>473</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5">
         <v>214</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="1">
         <f t="shared" si="3"/>
         <v>243</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="1">
         <f t="shared" si="4"/>
         <v>475</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="1">
         <f t="shared" si="5"/>
         <v>214</v>
       </c>
@@ -824,13 +822,13 @@
       <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6">
         <v>256</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6">
         <v>502</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6">
         <v>208</v>
       </c>
       <c r="F6">
@@ -842,24 +840,24 @@
       <c r="H6">
         <v>208</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6">
         <v>256</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6">
         <v>501</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6">
         <v>209</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6" s="1">
         <f t="shared" si="3"/>
         <v>256</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6" s="1">
         <f t="shared" si="4"/>
         <v>502</v>
       </c>
-      <c r="N6" s="2">
+      <c r="N6" s="1">
         <f t="shared" si="5"/>
         <v>208</v>
       </c>
@@ -907,13 +905,13 @@
       <c r="B7" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7">
         <v>797</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7">
         <v>524</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7">
         <v>247</v>
       </c>
       <c r="F7">
@@ -925,24 +923,24 @@
       <c r="H7">
         <v>247</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7">
         <v>795</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7">
         <v>524</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7">
         <v>246</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7" s="1">
         <f t="shared" si="3"/>
         <v>797</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7" s="1">
         <f t="shared" si="4"/>
         <v>524</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N7" s="1">
         <f t="shared" si="5"/>
         <v>247</v>
       </c>
@@ -990,13 +988,13 @@
       <c r="B8" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8">
         <v>782</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8">
         <v>542</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8">
         <v>232</v>
       </c>
       <c r="F8">
@@ -1008,24 +1006,24 @@
       <c r="H8">
         <v>232</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8">
         <v>780</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8">
         <v>542</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8">
         <v>231</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8" s="1">
         <f t="shared" si="3"/>
         <v>782</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M8" s="1">
         <f t="shared" si="4"/>
         <v>542</v>
       </c>
-      <c r="N8" s="2">
+      <c r="N8" s="1">
         <f t="shared" si="5"/>
         <v>232</v>
       </c>
@@ -1073,13 +1071,13 @@
       <c r="B9" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9">
         <v>246</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9">
         <v>486</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9">
         <v>223</v>
       </c>
       <c r="F9">
@@ -1091,24 +1089,24 @@
       <c r="H9">
         <v>223</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9">
         <v>245</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9">
         <v>485</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9">
         <v>224</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L9" s="1">
         <f t="shared" si="3"/>
         <v>246</v>
       </c>
-      <c r="M9" s="2">
+      <c r="M9" s="1">
         <f t="shared" si="4"/>
         <v>486</v>
       </c>
-      <c r="N9" s="2">
+      <c r="N9" s="1">
         <f t="shared" si="5"/>
         <v>223</v>
       </c>
@@ -1156,13 +1154,13 @@
       <c r="B10" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10">
         <v>255</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10">
         <v>508</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10">
         <v>210</v>
       </c>
       <c r="F10">
@@ -1174,24 +1172,24 @@
       <c r="H10">
         <v>210</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10">
         <v>256</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10">
         <v>508</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K10">
         <v>209</v>
       </c>
-      <c r="L10" s="2">
+      <c r="L10" s="1">
         <f t="shared" si="3"/>
         <v>255</v>
       </c>
-      <c r="M10" s="2">
+      <c r="M10" s="1">
         <f t="shared" si="4"/>
         <v>508</v>
       </c>
-      <c r="N10" s="2">
+      <c r="N10" s="1">
         <f t="shared" si="5"/>
         <v>210</v>
       </c>
@@ -1239,13 +1237,13 @@
       <c r="B11" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11">
         <v>809</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11">
         <v>588</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11">
         <v>278</v>
       </c>
       <c r="F11">
@@ -1257,24 +1255,24 @@
       <c r="H11">
         <v>278</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I11">
         <v>809</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11">
         <v>587</v>
       </c>
-      <c r="K11" s="1">
+      <c r="K11">
         <v>278</v>
       </c>
-      <c r="L11" s="2">
+      <c r="L11" s="1">
         <f t="shared" si="3"/>
         <v>809</v>
       </c>
-      <c r="M11" s="2">
+      <c r="M11" s="1">
         <f t="shared" si="4"/>
         <v>588</v>
       </c>
-      <c r="N11" s="2">
+      <c r="N11" s="1">
         <f t="shared" si="5"/>
         <v>278</v>
       </c>
@@ -1322,13 +1320,13 @@
       <c r="B12" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12">
         <v>800</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12">
         <v>610</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12">
         <v>262</v>
       </c>
       <c r="F12">
@@ -1340,24 +1338,24 @@
       <c r="H12">
         <v>262</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12">
         <v>797</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J12">
         <v>607</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K12">
         <v>261</v>
       </c>
-      <c r="L12" s="2">
+      <c r="L12" s="1">
         <f t="shared" si="3"/>
         <v>800</v>
       </c>
-      <c r="M12" s="2">
+      <c r="M12" s="1">
         <f t="shared" si="4"/>
         <v>610</v>
       </c>
-      <c r="N12" s="2">
+      <c r="N12" s="1">
         <f t="shared" si="5"/>
         <v>262</v>
       </c>
@@ -1405,13 +1403,13 @@
       <c r="B13" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13">
         <v>240</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13">
         <v>523</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13">
         <v>282</v>
       </c>
       <c r="F13">
@@ -1423,24 +1421,24 @@
       <c r="H13">
         <v>282</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13">
         <v>241</v>
       </c>
-      <c r="J13" s="1">
+      <c r="J13">
         <v>522</v>
       </c>
-      <c r="K13" s="1">
+      <c r="K13">
         <v>283</v>
       </c>
-      <c r="L13" s="2">
+      <c r="L13" s="1">
         <f t="shared" si="3"/>
         <v>240</v>
       </c>
-      <c r="M13" s="2">
+      <c r="M13" s="1">
         <f t="shared" si="4"/>
         <v>523</v>
       </c>
-      <c r="N13" s="2">
+      <c r="N13" s="1">
         <f t="shared" si="5"/>
         <v>282</v>
       </c>
@@ -1488,13 +1486,13 @@
       <c r="B14" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14">
         <v>246</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14">
         <v>548</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14">
         <v>264</v>
       </c>
       <c r="F14">
@@ -1506,24 +1504,24 @@
       <c r="H14">
         <v>264</v>
       </c>
-      <c r="I14" s="1">
+      <c r="I14">
         <v>245</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J14">
         <v>547</v>
       </c>
-      <c r="K14" s="1">
+      <c r="K14">
         <v>265</v>
       </c>
-      <c r="L14" s="2">
+      <c r="L14" s="1">
         <f t="shared" si="3"/>
         <v>246</v>
       </c>
-      <c r="M14" s="2">
+      <c r="M14" s="1">
         <f t="shared" si="4"/>
         <v>548</v>
       </c>
-      <c r="N14" s="2">
+      <c r="N14" s="1">
         <f t="shared" si="5"/>
         <v>264</v>
       </c>
@@ -1571,13 +1569,13 @@
       <c r="B15" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15">
         <v>795</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15">
         <v>438</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15">
         <v>240</v>
       </c>
       <c r="F15">
@@ -1589,24 +1587,24 @@
       <c r="H15">
         <v>239</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I15">
         <v>798</v>
       </c>
-      <c r="J15" s="1">
+      <c r="J15">
         <v>438</v>
       </c>
-      <c r="K15" s="1">
+      <c r="K15">
         <v>240</v>
       </c>
-      <c r="L15" s="2">
+      <c r="L15" s="1">
         <f t="shared" si="3"/>
         <v>795</v>
       </c>
-      <c r="M15" s="2">
+      <c r="M15" s="1">
         <f t="shared" si="4"/>
         <v>438</v>
       </c>
-      <c r="N15" s="2">
+      <c r="N15" s="1">
         <f t="shared" si="5"/>
         <v>240</v>
       </c>
@@ -1654,13 +1652,13 @@
       <c r="B16" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16">
         <v>786</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16">
         <v>459</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16">
         <v>225</v>
       </c>
       <c r="F16">
@@ -1672,24 +1670,24 @@
       <c r="H16">
         <v>226</v>
       </c>
-      <c r="I16" s="1">
+      <c r="I16">
         <v>785</v>
       </c>
-      <c r="J16" s="1">
+      <c r="J16">
         <v>458</v>
       </c>
-      <c r="K16" s="1">
+      <c r="K16">
         <v>225</v>
       </c>
-      <c r="L16" s="2">
+      <c r="L16" s="1">
         <f t="shared" si="3"/>
         <v>786</v>
       </c>
-      <c r="M16" s="2">
+      <c r="M16" s="1">
         <f t="shared" si="4"/>
         <v>459</v>
       </c>
-      <c r="N16" s="2">
+      <c r="N16" s="1">
         <f t="shared" si="5"/>
         <v>225</v>
       </c>
@@ -1737,13 +1735,13 @@
       <c r="B17" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17">
         <v>248</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17">
         <v>364</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17">
         <v>269</v>
       </c>
       <c r="F17">
@@ -1755,24 +1753,24 @@
       <c r="H17">
         <v>269</v>
       </c>
-      <c r="I17" s="1">
+      <c r="I17">
         <v>250</v>
       </c>
-      <c r="J17" s="1">
+      <c r="J17">
         <v>364</v>
       </c>
-      <c r="K17" s="1">
+      <c r="K17">
         <v>269</v>
       </c>
-      <c r="L17" s="2">
+      <c r="L17" s="1">
         <f t="shared" si="3"/>
         <v>248</v>
       </c>
-      <c r="M17" s="2">
+      <c r="M17" s="1">
         <f t="shared" si="4"/>
         <v>364</v>
       </c>
-      <c r="N17" s="2">
+      <c r="N17" s="1">
         <f t="shared" si="5"/>
         <v>269</v>
       </c>
@@ -1820,13 +1818,13 @@
       <c r="B18" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18">
         <v>255</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18">
         <v>388</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18">
         <v>254</v>
       </c>
       <c r="F18">
@@ -1838,24 +1836,24 @@
       <c r="H18">
         <v>254</v>
       </c>
-      <c r="I18" s="1">
+      <c r="I18">
         <v>256</v>
       </c>
-      <c r="J18" s="1">
+      <c r="J18">
         <v>388</v>
       </c>
-      <c r="K18" s="1">
+      <c r="K18">
         <v>255</v>
       </c>
-      <c r="L18" s="2">
+      <c r="L18" s="1">
         <f t="shared" si="3"/>
         <v>255</v>
       </c>
-      <c r="M18" s="2">
+      <c r="M18" s="1">
         <f t="shared" si="4"/>
         <v>388</v>
       </c>
-      <c r="N18" s="2">
+      <c r="N18" s="1">
         <f t="shared" si="5"/>
         <v>254</v>
       </c>
@@ -1903,13 +1901,13 @@
       <c r="B19" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19">
         <v>817</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19">
         <v>399</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19">
         <v>216</v>
       </c>
       <c r="F19">
@@ -1921,24 +1919,24 @@
       <c r="H19">
         <v>216</v>
       </c>
-      <c r="I19" s="1">
+      <c r="I19">
         <v>817</v>
       </c>
-      <c r="J19" s="1">
+      <c r="J19">
         <v>399</v>
       </c>
-      <c r="K19" s="1">
+      <c r="K19">
         <v>217</v>
       </c>
-      <c r="L19" s="2">
+      <c r="L19" s="1">
         <f t="shared" si="3"/>
         <v>817</v>
       </c>
-      <c r="M19" s="2">
+      <c r="M19" s="1">
         <f t="shared" si="4"/>
         <v>399</v>
       </c>
-      <c r="N19" s="2">
+      <c r="N19" s="1">
         <f t="shared" si="5"/>
         <v>216</v>
       </c>
@@ -1986,13 +1984,13 @@
       <c r="B20" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20">
         <v>808</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20">
         <v>427</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20">
         <v>206</v>
       </c>
       <c r="F20">
@@ -2004,24 +2002,24 @@
       <c r="H20">
         <v>206</v>
       </c>
-      <c r="I20" s="1">
+      <c r="I20">
         <v>807</v>
       </c>
-      <c r="J20" s="1">
+      <c r="J20">
         <v>426</v>
       </c>
-      <c r="K20" s="1">
+      <c r="K20">
         <v>207</v>
       </c>
-      <c r="L20" s="2">
+      <c r="L20" s="1">
         <f t="shared" si="3"/>
         <v>808</v>
       </c>
-      <c r="M20" s="2">
+      <c r="M20" s="1">
         <f t="shared" si="4"/>
         <v>427</v>
       </c>
-      <c r="N20" s="2">
+      <c r="N20" s="1">
         <f t="shared" si="5"/>
         <v>206</v>
       </c>
@@ -2069,13 +2067,13 @@
       <c r="B21" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21">
         <v>246</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21">
         <v>413</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21">
         <v>241</v>
       </c>
       <c r="F21">
@@ -2087,24 +2085,24 @@
       <c r="H21">
         <v>241</v>
       </c>
-      <c r="I21" s="1">
+      <c r="I21">
         <v>247</v>
       </c>
-      <c r="J21" s="1">
+      <c r="J21">
         <v>412</v>
       </c>
-      <c r="K21" s="1">
+      <c r="K21">
         <v>243</v>
       </c>
-      <c r="L21" s="2">
+      <c r="L21" s="1">
         <f t="shared" si="3"/>
         <v>246</v>
       </c>
-      <c r="M21" s="2">
+      <c r="M21" s="1">
         <f t="shared" si="4"/>
         <v>413</v>
       </c>
-      <c r="N21" s="2">
+      <c r="N21" s="1">
         <f t="shared" si="5"/>
         <v>241</v>
       </c>
@@ -2152,13 +2150,13 @@
       <c r="B22" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22">
         <v>261</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22">
         <v>433</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22">
         <v>235</v>
       </c>
       <c r="F22">
@@ -2170,24 +2168,24 @@
       <c r="H22">
         <v>235</v>
       </c>
-      <c r="I22" s="1">
+      <c r="I22">
         <v>259</v>
       </c>
-      <c r="J22" s="1">
+      <c r="J22">
         <v>435</v>
       </c>
-      <c r="K22" s="1">
+      <c r="K22">
         <v>235</v>
       </c>
-      <c r="L22" s="2">
+      <c r="L22" s="1">
         <f t="shared" si="3"/>
         <v>261</v>
       </c>
-      <c r="M22" s="2">
+      <c r="M22" s="1">
         <f t="shared" si="4"/>
         <v>433</v>
       </c>
-      <c r="N22" s="2">
+      <c r="N22" s="1">
         <f t="shared" si="5"/>
         <v>235</v>
       </c>
@@ -2235,13 +2233,13 @@
       <c r="B23" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23">
         <v>778</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23">
         <v>519</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23">
         <v>215</v>
       </c>
       <c r="F23">
@@ -2253,24 +2251,24 @@
       <c r="H23">
         <v>215</v>
       </c>
-      <c r="I23" s="1">
+      <c r="I23">
         <v>780</v>
       </c>
-      <c r="J23" s="1">
+      <c r="J23">
         <v>520</v>
       </c>
-      <c r="K23" s="1">
+      <c r="K23">
         <v>214</v>
       </c>
-      <c r="L23" s="2">
+      <c r="L23" s="1">
         <f t="shared" si="3"/>
         <v>778</v>
       </c>
-      <c r="M23" s="2">
+      <c r="M23" s="1">
         <f t="shared" si="4"/>
         <v>519</v>
       </c>
-      <c r="N23" s="2">
+      <c r="N23" s="1">
         <f t="shared" si="5"/>
         <v>215</v>
       </c>
@@ -2318,13 +2316,13 @@
       <c r="B24" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24">
         <v>771</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24">
         <v>547</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E24">
         <v>206</v>
       </c>
       <c r="F24">
@@ -2336,24 +2334,24 @@
       <c r="H24">
         <v>206</v>
       </c>
-      <c r="I24" s="1">
+      <c r="I24">
         <v>768</v>
       </c>
-      <c r="J24" s="1">
+      <c r="J24">
         <v>547</v>
       </c>
-      <c r="K24" s="1">
+      <c r="K24">
         <v>206</v>
       </c>
-      <c r="L24" s="2">
+      <c r="L24" s="1">
         <f t="shared" si="3"/>
         <v>771</v>
       </c>
-      <c r="M24" s="2">
+      <c r="M24" s="1">
         <f t="shared" si="4"/>
         <v>547</v>
       </c>
-      <c r="N24" s="2">
+      <c r="N24" s="1">
         <f t="shared" si="5"/>
         <v>206</v>
       </c>
@@ -2401,13 +2399,13 @@
       <c r="B25" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25">
         <v>277</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25">
         <v>534</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E25">
         <v>176</v>
       </c>
       <c r="F25">
@@ -2419,24 +2417,24 @@
       <c r="H25">
         <v>176</v>
       </c>
-      <c r="I25" s="1">
+      <c r="I25">
         <v>278</v>
       </c>
-      <c r="J25" s="1">
+      <c r="J25">
         <v>532</v>
       </c>
-      <c r="K25" s="1">
+      <c r="K25">
         <v>179</v>
       </c>
-      <c r="L25" s="2">
+      <c r="L25" s="1">
         <f t="shared" si="3"/>
         <v>277</v>
       </c>
-      <c r="M25" s="2">
+      <c r="M25" s="1">
         <f t="shared" si="4"/>
         <v>534</v>
       </c>
-      <c r="N25" s="2">
+      <c r="N25" s="1">
         <f t="shared" si="5"/>
         <v>176</v>
       </c>
@@ -2484,13 +2482,13 @@
       <c r="B26" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26">
         <v>287</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26">
         <v>561</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E26">
         <v>169</v>
       </c>
       <c r="F26">
@@ -2502,24 +2500,24 @@
       <c r="H26">
         <v>169</v>
       </c>
-      <c r="I26" s="1">
+      <c r="I26">
         <v>289</v>
       </c>
-      <c r="J26" s="1">
+      <c r="J26">
         <v>559</v>
       </c>
-      <c r="K26" s="1">
+      <c r="K26">
         <v>169</v>
       </c>
-      <c r="L26" s="2">
+      <c r="L26" s="1">
         <f t="shared" si="3"/>
         <v>287</v>
       </c>
-      <c r="M26" s="2">
+      <c r="M26" s="1">
         <f t="shared" si="4"/>
         <v>561</v>
       </c>
-      <c r="N26" s="2">
+      <c r="N26" s="1">
         <f t="shared" si="5"/>
         <v>169</v>
       </c>
@@ -2567,13 +2565,13 @@
       <c r="B27" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27">
         <v>779</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27">
         <v>523</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E27">
         <v>232</v>
       </c>
       <c r="F27">
@@ -2585,24 +2583,24 @@
       <c r="H27">
         <v>232</v>
       </c>
-      <c r="I27" s="1">
+      <c r="I27">
         <v>778</v>
       </c>
-      <c r="J27" s="1">
+      <c r="J27">
         <v>522</v>
       </c>
-      <c r="K27" s="1">
+      <c r="K27">
         <v>232</v>
       </c>
-      <c r="L27" s="2">
+      <c r="L27" s="1">
         <f t="shared" si="3"/>
         <v>779</v>
       </c>
-      <c r="M27" s="2">
+      <c r="M27" s="1">
         <f t="shared" si="4"/>
         <v>523</v>
       </c>
-      <c r="N27" s="2">
+      <c r="N27" s="1">
         <f t="shared" si="5"/>
         <v>232</v>
       </c>
@@ -2650,13 +2648,13 @@
       <c r="B28" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28">
         <v>765</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28">
         <v>544</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E28">
         <v>222</v>
       </c>
       <c r="F28">
@@ -2668,24 +2666,24 @@
       <c r="H28">
         <v>222</v>
       </c>
-      <c r="I28" s="1">
+      <c r="I28">
         <v>764</v>
       </c>
-      <c r="J28" s="1">
+      <c r="J28">
         <v>544</v>
       </c>
-      <c r="K28" s="1">
+      <c r="K28">
         <v>223</v>
       </c>
-      <c r="L28" s="2">
+      <c r="L28" s="1">
         <f t="shared" si="3"/>
         <v>765</v>
       </c>
-      <c r="M28" s="2">
+      <c r="M28" s="1">
         <f t="shared" si="4"/>
         <v>544</v>
       </c>
-      <c r="N28" s="2">
+      <c r="N28" s="1">
         <f t="shared" si="5"/>
         <v>222</v>
       </c>
@@ -2733,13 +2731,13 @@
       <c r="B29" t="s">
         <v>3</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29">
         <v>271</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29">
         <v>488</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E29">
         <v>227</v>
       </c>
       <c r="F29">
@@ -2751,24 +2749,24 @@
       <c r="H29">
         <v>227</v>
       </c>
-      <c r="I29" s="1">
+      <c r="I29">
         <v>270</v>
       </c>
-      <c r="J29" s="1">
+      <c r="J29">
         <v>487</v>
       </c>
-      <c r="K29" s="1">
+      <c r="K29">
         <v>228</v>
       </c>
-      <c r="L29" s="2">
+      <c r="L29" s="1">
         <f t="shared" si="3"/>
         <v>271</v>
       </c>
-      <c r="M29" s="2">
+      <c r="M29" s="1">
         <f t="shared" si="4"/>
         <v>488</v>
       </c>
-      <c r="N29" s="2">
+      <c r="N29" s="1">
         <f t="shared" si="5"/>
         <v>227</v>
       </c>
@@ -2816,13 +2814,13 @@
       <c r="B30" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30">
         <v>279</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30">
         <v>512</v>
       </c>
-      <c r="E30" s="1">
+      <c r="E30">
         <v>219</v>
       </c>
       <c r="F30">
@@ -2834,24 +2832,24 @@
       <c r="H30">
         <v>219</v>
       </c>
-      <c r="I30" s="1">
+      <c r="I30">
         <v>280</v>
       </c>
-      <c r="J30" s="1">
+      <c r="J30">
         <v>514</v>
       </c>
-      <c r="K30" s="1">
+      <c r="K30">
         <v>220</v>
       </c>
-      <c r="L30" s="2">
+      <c r="L30" s="1">
         <f t="shared" si="3"/>
         <v>279</v>
       </c>
-      <c r="M30" s="2">
+      <c r="M30" s="1">
         <f t="shared" si="4"/>
         <v>512</v>
       </c>
-      <c r="N30" s="2">
+      <c r="N30" s="1">
         <f t="shared" si="5"/>
         <v>219</v>
       </c>
@@ -2899,13 +2897,13 @@
       <c r="B31" t="s">
         <v>1</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31">
         <v>805</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31">
         <v>513</v>
       </c>
-      <c r="E31" s="1">
+      <c r="E31">
         <v>247</v>
       </c>
       <c r="F31">
@@ -2917,24 +2915,24 @@
       <c r="H31">
         <v>247</v>
       </c>
-      <c r="I31" s="1">
+      <c r="I31">
         <v>807</v>
       </c>
-      <c r="J31" s="1">
+      <c r="J31">
         <v>513</v>
       </c>
-      <c r="K31" s="1">
+      <c r="K31">
         <v>247</v>
       </c>
-      <c r="L31" s="2">
+      <c r="L31" s="1">
         <f t="shared" si="3"/>
         <v>805</v>
       </c>
-      <c r="M31" s="2">
+      <c r="M31" s="1">
         <f t="shared" si="4"/>
         <v>513</v>
       </c>
-      <c r="N31" s="2">
+      <c r="N31" s="1">
         <f t="shared" si="5"/>
         <v>247</v>
       </c>
@@ -2982,13 +2980,13 @@
       <c r="B32" t="s">
         <v>2</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32">
         <v>795</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32">
         <v>535</v>
       </c>
-      <c r="E32" s="1">
+      <c r="E32">
         <v>233</v>
       </c>
       <c r="F32">
@@ -3000,24 +2998,24 @@
       <c r="H32">
         <v>233</v>
       </c>
-      <c r="I32" s="1">
+      <c r="I32">
         <v>794</v>
       </c>
-      <c r="J32" s="1">
+      <c r="J32">
         <v>535</v>
       </c>
-      <c r="K32" s="1">
+      <c r="K32">
         <v>232</v>
       </c>
-      <c r="L32" s="2">
+      <c r="L32" s="1">
         <f t="shared" si="3"/>
         <v>795</v>
       </c>
-      <c r="M32" s="2">
+      <c r="M32" s="1">
         <f t="shared" si="4"/>
         <v>535</v>
       </c>
-      <c r="N32" s="2">
+      <c r="N32" s="1">
         <f t="shared" si="5"/>
         <v>233</v>
       </c>
@@ -3065,13 +3063,13 @@
       <c r="B33" t="s">
         <v>3</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33">
         <v>245</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D33">
         <v>529</v>
       </c>
-      <c r="E33" s="1">
+      <c r="E33">
         <v>209</v>
       </c>
       <c r="F33">
@@ -3083,24 +3081,24 @@
       <c r="H33">
         <v>209</v>
       </c>
-      <c r="I33" s="1">
+      <c r="I33">
         <v>245</v>
       </c>
-      <c r="J33" s="1">
+      <c r="J33">
         <v>531</v>
       </c>
-      <c r="K33" s="1">
+      <c r="K33">
         <v>209</v>
       </c>
-      <c r="L33" s="2">
+      <c r="L33" s="1">
         <f t="shared" si="3"/>
         <v>245</v>
       </c>
-      <c r="M33" s="2">
+      <c r="M33" s="1">
         <f t="shared" si="4"/>
         <v>529</v>
       </c>
-      <c r="N33" s="2">
+      <c r="N33" s="1">
         <f t="shared" si="5"/>
         <v>209</v>
       </c>
@@ -3148,13 +3146,13 @@
       <c r="B34" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C34">
         <v>261</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D34">
         <v>550</v>
       </c>
-      <c r="E34" s="1">
+      <c r="E34">
         <v>197</v>
       </c>
       <c r="F34">
@@ -3166,24 +3164,24 @@
       <c r="H34">
         <v>197</v>
       </c>
-      <c r="I34" s="1">
+      <c r="I34">
         <v>261</v>
       </c>
-      <c r="J34" s="1">
+      <c r="J34">
         <v>552</v>
       </c>
-      <c r="K34" s="1">
+      <c r="K34">
         <v>198</v>
       </c>
-      <c r="L34" s="2">
+      <c r="L34" s="1">
         <f t="shared" si="3"/>
         <v>261</v>
       </c>
-      <c r="M34" s="2">
+      <c r="M34" s="1">
         <f t="shared" si="4"/>
         <v>550</v>
       </c>
-      <c r="N34" s="2">
+      <c r="N34" s="1">
         <f t="shared" si="5"/>
         <v>197</v>
       </c>
@@ -3231,13 +3229,13 @@
       <c r="B35" t="s">
         <v>1</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35">
         <v>769</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D35">
         <v>526</v>
       </c>
-      <c r="E35" s="1">
+      <c r="E35">
         <v>246</v>
       </c>
       <c r="F35">
@@ -3249,24 +3247,24 @@
       <c r="H35">
         <v>246</v>
       </c>
-      <c r="I35" s="1">
+      <c r="I35">
         <v>768</v>
       </c>
-      <c r="J35" s="1">
+      <c r="J35">
         <v>525</v>
       </c>
-      <c r="K35" s="1">
+      <c r="K35">
         <v>247</v>
       </c>
-      <c r="L35" s="2">
+      <c r="L35" s="1">
         <f t="shared" si="3"/>
         <v>769</v>
       </c>
-      <c r="M35" s="2">
+      <c r="M35" s="1">
         <f t="shared" si="4"/>
         <v>526</v>
       </c>
-      <c r="N35" s="2">
+      <c r="N35" s="1">
         <f t="shared" si="5"/>
         <v>246</v>
       </c>
@@ -3314,13 +3312,13 @@
       <c r="B36" t="s">
         <v>2</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36">
         <v>761</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D36">
         <v>545</v>
       </c>
-      <c r="E36" s="1">
+      <c r="E36">
         <v>238</v>
       </c>
       <c r="F36">
@@ -3332,24 +3330,24 @@
       <c r="H36">
         <v>238</v>
       </c>
-      <c r="I36" s="1">
+      <c r="I36">
         <v>758</v>
       </c>
-      <c r="J36" s="1">
+      <c r="J36">
         <v>543</v>
       </c>
-      <c r="K36" s="1">
+      <c r="K36">
         <v>239</v>
       </c>
-      <c r="L36" s="2">
+      <c r="L36" s="1">
         <f t="shared" si="3"/>
         <v>761</v>
       </c>
-      <c r="M36" s="2">
+      <c r="M36" s="1">
         <f t="shared" si="4"/>
         <v>545</v>
       </c>
-      <c r="N36" s="2">
+      <c r="N36" s="1">
         <f t="shared" si="5"/>
         <v>238</v>
       </c>
@@ -3397,13 +3395,13 @@
       <c r="B37" t="s">
         <v>3</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C37">
         <v>220</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D37">
         <v>528</v>
       </c>
-      <c r="E37" s="1">
+      <c r="E37">
         <v>271</v>
       </c>
       <c r="F37">
@@ -3415,24 +3413,24 @@
       <c r="H37">
         <v>271</v>
       </c>
-      <c r="I37" s="1">
+      <c r="I37">
         <v>220</v>
       </c>
-      <c r="J37" s="1">
+      <c r="J37">
         <v>527</v>
       </c>
-      <c r="K37" s="1">
+      <c r="K37">
         <v>272</v>
       </c>
-      <c r="L37" s="2">
+      <c r="L37" s="1">
         <f t="shared" si="3"/>
         <v>220</v>
       </c>
-      <c r="M37" s="2">
+      <c r="M37" s="1">
         <f t="shared" si="4"/>
         <v>528</v>
       </c>
-      <c r="N37" s="2">
+      <c r="N37" s="1">
         <f t="shared" si="5"/>
         <v>271</v>
       </c>
@@ -3480,13 +3478,13 @@
       <c r="B38" t="s">
         <v>4</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C38">
         <v>225</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D38">
         <v>546</v>
       </c>
-      <c r="E38" s="1">
+      <c r="E38">
         <v>263</v>
       </c>
       <c r="F38">
@@ -3498,24 +3496,24 @@
       <c r="H38">
         <v>263</v>
       </c>
-      <c r="I38" s="1">
+      <c r="I38">
         <v>227</v>
       </c>
-      <c r="J38" s="1">
+      <c r="J38">
         <v>545</v>
       </c>
-      <c r="K38" s="1">
+      <c r="K38">
         <v>263</v>
       </c>
-      <c r="L38" s="2">
+      <c r="L38" s="1">
         <f t="shared" si="3"/>
         <v>225</v>
       </c>
-      <c r="M38" s="2">
+      <c r="M38" s="1">
         <f t="shared" si="4"/>
         <v>546</v>
       </c>
-      <c r="N38" s="2">
+      <c r="N38" s="1">
         <f t="shared" si="5"/>
         <v>263</v>
       </c>
@@ -3563,13 +3561,13 @@
       <c r="B39" t="s">
         <v>1</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C39">
         <v>812</v>
       </c>
-      <c r="D39" s="1">
+      <c r="D39">
         <v>444</v>
       </c>
-      <c r="E39" s="1">
+      <c r="E39">
         <v>262</v>
       </c>
       <c r="F39">
@@ -3581,24 +3579,24 @@
       <c r="H39">
         <v>262</v>
       </c>
-      <c r="I39" s="1">
+      <c r="I39">
         <v>810</v>
       </c>
-      <c r="J39" s="1">
+      <c r="J39">
         <v>445</v>
       </c>
-      <c r="K39" s="1">
+      <c r="K39">
         <v>262</v>
       </c>
-      <c r="L39" s="2">
+      <c r="L39" s="1">
         <f t="shared" si="3"/>
         <v>812</v>
       </c>
-      <c r="M39" s="2">
+      <c r="M39" s="1">
         <f t="shared" si="4"/>
         <v>444</v>
       </c>
-      <c r="N39" s="2">
+      <c r="N39" s="1">
         <f t="shared" si="5"/>
         <v>262</v>
       </c>
@@ -3646,13 +3644,13 @@
       <c r="B40" t="s">
         <v>2</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C40">
         <v>802</v>
       </c>
-      <c r="D40" s="1">
+      <c r="D40">
         <v>473</v>
       </c>
-      <c r="E40" s="1">
+      <c r="E40">
         <v>251</v>
       </c>
       <c r="F40">
@@ -3664,24 +3662,24 @@
       <c r="H40">
         <v>251</v>
       </c>
-      <c r="I40" s="1">
+      <c r="I40">
         <v>800</v>
       </c>
-      <c r="J40" s="1">
+      <c r="J40">
         <v>470</v>
       </c>
-      <c r="K40" s="1">
+      <c r="K40">
         <v>252</v>
       </c>
-      <c r="L40" s="2">
+      <c r="L40" s="1">
         <f t="shared" si="3"/>
         <v>802</v>
       </c>
-      <c r="M40" s="2">
+      <c r="M40" s="1">
         <f t="shared" si="4"/>
         <v>473</v>
       </c>
-      <c r="N40" s="2">
+      <c r="N40" s="1">
         <f t="shared" si="5"/>
         <v>251</v>
       </c>
@@ -3729,13 +3727,13 @@
       <c r="B41" t="s">
         <v>3</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C41">
         <v>215</v>
       </c>
-      <c r="D41" s="1">
+      <c r="D41">
         <v>464</v>
       </c>
-      <c r="E41" s="1">
+      <c r="E41">
         <v>244</v>
       </c>
       <c r="F41">
@@ -3747,24 +3745,24 @@
       <c r="H41">
         <v>244</v>
       </c>
-      <c r="I41" s="1">
+      <c r="I41">
         <v>215</v>
       </c>
-      <c r="J41" s="1">
+      <c r="J41">
         <v>464</v>
       </c>
-      <c r="K41" s="1">
+      <c r="K41">
         <v>244</v>
       </c>
-      <c r="L41" s="2">
+      <c r="L41" s="1">
         <f t="shared" si="3"/>
         <v>215</v>
       </c>
-      <c r="M41" s="2">
+      <c r="M41" s="1">
         <f t="shared" si="4"/>
         <v>464</v>
       </c>
-      <c r="N41" s="2">
+      <c r="N41" s="1">
         <f t="shared" si="5"/>
         <v>244</v>
       </c>
@@ -3812,13 +3810,13 @@
       <c r="B42" t="s">
         <v>4</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42">
         <v>228</v>
       </c>
-      <c r="D42" s="1">
+      <c r="D42">
         <v>486</v>
       </c>
-      <c r="E42" s="1">
+      <c r="E42">
         <v>231</v>
       </c>
       <c r="F42">
@@ -3830,24 +3828,24 @@
       <c r="H42">
         <v>231</v>
       </c>
-      <c r="I42" s="1">
+      <c r="I42">
         <v>226</v>
       </c>
-      <c r="J42" s="1">
+      <c r="J42">
         <v>488</v>
       </c>
-      <c r="K42" s="1">
+      <c r="K42">
         <v>232</v>
       </c>
-      <c r="L42" s="2">
+      <c r="L42" s="1">
         <f t="shared" si="3"/>
         <v>228</v>
       </c>
-      <c r="M42" s="2">
+      <c r="M42" s="1">
         <f t="shared" si="4"/>
         <v>486</v>
       </c>
-      <c r="N42" s="2">
+      <c r="N42" s="1">
         <f t="shared" si="5"/>
         <v>231</v>
       </c>
@@ -3895,13 +3893,13 @@
       <c r="B43" t="s">
         <v>1</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43">
         <v>784</v>
       </c>
-      <c r="D43" s="1">
+      <c r="D43">
         <v>523</v>
       </c>
-      <c r="E43" s="1">
+      <c r="E43">
         <v>232</v>
       </c>
       <c r="F43">
@@ -3913,24 +3911,24 @@
       <c r="H43">
         <v>232</v>
       </c>
-      <c r="I43" s="1">
+      <c r="I43">
         <v>784</v>
       </c>
-      <c r="J43" s="1">
+      <c r="J43">
         <v>523</v>
       </c>
-      <c r="K43" s="1">
+      <c r="K43">
         <v>233</v>
       </c>
-      <c r="L43" s="2">
+      <c r="L43" s="1">
         <f t="shared" si="3"/>
         <v>784</v>
       </c>
-      <c r="M43" s="2">
+      <c r="M43" s="1">
         <f t="shared" si="4"/>
         <v>523</v>
       </c>
-      <c r="N43" s="2">
+      <c r="N43" s="1">
         <f t="shared" si="5"/>
         <v>232</v>
       </c>
@@ -3978,13 +3976,13 @@
       <c r="B44" t="s">
         <v>2</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44">
         <v>773</v>
       </c>
-      <c r="D44" s="1">
+      <c r="D44">
         <v>547</v>
       </c>
-      <c r="E44" s="1">
+      <c r="E44">
         <v>221</v>
       </c>
       <c r="F44">
@@ -3996,24 +3994,24 @@
       <c r="H44">
         <v>221</v>
       </c>
-      <c r="I44" s="1">
+      <c r="I44">
         <v>771</v>
       </c>
-      <c r="J44" s="1">
+      <c r="J44">
         <v>545</v>
       </c>
-      <c r="K44" s="1">
+      <c r="K44">
         <v>222</v>
       </c>
-      <c r="L44" s="2">
+      <c r="L44" s="1">
         <f t="shared" si="3"/>
         <v>773</v>
       </c>
-      <c r="M44" s="2">
+      <c r="M44" s="1">
         <f t="shared" si="4"/>
         <v>547</v>
       </c>
-      <c r="N44" s="2">
+      <c r="N44" s="1">
         <f t="shared" si="5"/>
         <v>221</v>
       </c>
@@ -4061,13 +4059,13 @@
       <c r="B45" t="s">
         <v>3</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45">
         <v>233</v>
       </c>
-      <c r="D45" s="1">
+      <c r="D45">
         <v>484</v>
       </c>
-      <c r="E45" s="1">
+      <c r="E45">
         <v>260</v>
       </c>
       <c r="F45">
@@ -4079,24 +4077,24 @@
       <c r="H45">
         <v>260</v>
       </c>
-      <c r="I45" s="1">
+      <c r="I45">
         <v>235</v>
       </c>
-      <c r="J45" s="1">
+      <c r="J45">
         <v>484</v>
       </c>
-      <c r="K45" s="1">
+      <c r="K45">
         <v>259</v>
       </c>
-      <c r="L45" s="2">
+      <c r="L45" s="1">
         <f t="shared" si="3"/>
         <v>233</v>
       </c>
-      <c r="M45" s="2">
+      <c r="M45" s="1">
         <f t="shared" si="4"/>
         <v>484</v>
       </c>
-      <c r="N45" s="2">
+      <c r="N45" s="1">
         <f t="shared" si="5"/>
         <v>260</v>
       </c>
@@ -4144,13 +4142,13 @@
       <c r="B46" t="s">
         <v>4</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C46">
         <v>243</v>
       </c>
-      <c r="D46" s="1">
+      <c r="D46">
         <v>508</v>
       </c>
-      <c r="E46" s="1">
+      <c r="E46">
         <v>246</v>
       </c>
       <c r="F46">
@@ -4162,24 +4160,24 @@
       <c r="H46">
         <v>246</v>
       </c>
-      <c r="I46" s="1">
+      <c r="I46">
         <v>244</v>
       </c>
-      <c r="J46" s="1">
+      <c r="J46">
         <v>507</v>
       </c>
-      <c r="K46" s="1">
+      <c r="K46">
         <v>247</v>
       </c>
-      <c r="L46" s="2">
+      <c r="L46" s="1">
         <f t="shared" si="3"/>
         <v>243</v>
       </c>
-      <c r="M46" s="2">
+      <c r="M46" s="1">
         <f t="shared" si="4"/>
         <v>508</v>
       </c>
-      <c r="N46" s="2">
+      <c r="N46" s="1">
         <f t="shared" si="5"/>
         <v>246</v>
       </c>
@@ -4227,13 +4225,13 @@
       <c r="B47" t="s">
         <v>1</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47">
         <v>800</v>
       </c>
-      <c r="D47" s="1">
+      <c r="D47">
         <v>425</v>
       </c>
-      <c r="E47" s="1">
+      <c r="E47">
         <v>274</v>
       </c>
       <c r="F47">
@@ -4245,24 +4243,24 @@
       <c r="H47">
         <v>273</v>
       </c>
-      <c r="I47" s="1">
+      <c r="I47">
         <v>800</v>
       </c>
-      <c r="J47" s="1">
+      <c r="J47">
         <v>424</v>
       </c>
-      <c r="K47" s="1">
+      <c r="K47">
         <v>274</v>
       </c>
-      <c r="L47" s="2">
+      <c r="L47" s="1">
         <f t="shared" si="3"/>
         <v>800</v>
       </c>
-      <c r="M47" s="2">
+      <c r="M47" s="1">
         <f t="shared" si="4"/>
         <v>425</v>
       </c>
-      <c r="N47" s="2">
+      <c r="N47" s="1">
         <f t="shared" si="5"/>
         <v>274</v>
       </c>
@@ -4310,13 +4308,13 @@
       <c r="B48" t="s">
         <v>2</v>
       </c>
-      <c r="C48" s="1">
+      <c r="C48">
         <v>791</v>
       </c>
-      <c r="D48" s="1">
+      <c r="D48">
         <v>453</v>
       </c>
-      <c r="E48" s="1">
+      <c r="E48">
         <v>264</v>
       </c>
       <c r="F48">
@@ -4328,24 +4326,24 @@
       <c r="H48">
         <v>264</v>
       </c>
-      <c r="I48" s="1">
+      <c r="I48">
         <v>790</v>
       </c>
-      <c r="J48" s="1">
+      <c r="J48">
         <v>452</v>
       </c>
-      <c r="K48" s="1">
+      <c r="K48">
         <v>274</v>
       </c>
-      <c r="L48" s="2">
+      <c r="L48" s="1">
         <f t="shared" si="3"/>
         <v>791</v>
       </c>
-      <c r="M48" s="2">
+      <c r="M48" s="1">
         <f t="shared" si="4"/>
         <v>453</v>
       </c>
-      <c r="N48" s="2">
+      <c r="N48" s="1">
         <f t="shared" si="5"/>
         <v>264</v>
       </c>
@@ -4393,13 +4391,13 @@
       <c r="B49" t="s">
         <v>3</v>
       </c>
-      <c r="C49" s="1">
+      <c r="C49">
         <v>202</v>
       </c>
-      <c r="D49" s="1">
+      <c r="D49">
         <v>419</v>
       </c>
-      <c r="E49" s="1">
+      <c r="E49">
         <v>243</v>
       </c>
       <c r="F49">
@@ -4411,24 +4409,24 @@
       <c r="H49">
         <v>242</v>
       </c>
-      <c r="I49" s="1">
+      <c r="I49">
         <v>203</v>
       </c>
-      <c r="J49" s="1">
+      <c r="J49">
         <v>418</v>
       </c>
-      <c r="K49" s="1">
+      <c r="K49">
         <v>243</v>
       </c>
-      <c r="L49" s="2">
+      <c r="L49" s="1">
         <f t="shared" si="3"/>
         <v>202</v>
       </c>
-      <c r="M49" s="2">
+      <c r="M49" s="1">
         <f t="shared" si="4"/>
         <v>419</v>
       </c>
-      <c r="N49" s="2">
+      <c r="N49" s="1">
         <f t="shared" si="5"/>
         <v>243</v>
       </c>
@@ -4476,13 +4474,13 @@
       <c r="B50" t="s">
         <v>4</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C50">
         <v>216</v>
       </c>
-      <c r="D50" s="1">
+      <c r="D50">
         <v>445</v>
       </c>
-      <c r="E50" s="1">
+      <c r="E50">
         <v>232</v>
       </c>
       <c r="F50">
@@ -4494,24 +4492,24 @@
       <c r="H50">
         <v>233</v>
       </c>
-      <c r="I50" s="1">
+      <c r="I50">
         <v>214</v>
       </c>
-      <c r="J50" s="1">
+      <c r="J50">
         <v>448</v>
       </c>
-      <c r="K50" s="1">
+      <c r="K50">
         <v>233</v>
       </c>
-      <c r="L50" s="2">
+      <c r="L50" s="1">
         <f t="shared" si="3"/>
         <v>214</v>
       </c>
-      <c r="M50" s="2">
+      <c r="M50" s="1">
         <f t="shared" si="4"/>
         <v>448</v>
       </c>
-      <c r="N50" s="2">
+      <c r="N50" s="1">
         <f t="shared" si="5"/>
         <v>233</v>
       </c>
@@ -4559,13 +4557,13 @@
       <c r="B51" t="s">
         <v>1</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C51">
         <v>795</v>
       </c>
-      <c r="D51" s="1">
+      <c r="D51">
         <v>519</v>
       </c>
-      <c r="E51" s="1">
+      <c r="E51">
         <v>209</v>
       </c>
       <c r="F51">
@@ -4577,24 +4575,24 @@
       <c r="H51">
         <v>210</v>
       </c>
-      <c r="I51" s="1">
+      <c r="I51">
         <v>794</v>
       </c>
-      <c r="J51" s="1">
+      <c r="J51">
         <v>518</v>
       </c>
-      <c r="K51" s="1">
+      <c r="K51">
         <v>210</v>
       </c>
-      <c r="L51" s="2">
+      <c r="L51" s="1">
         <f t="shared" si="3"/>
         <v>795</v>
       </c>
-      <c r="M51" s="2">
+      <c r="M51" s="1">
         <f t="shared" si="4"/>
         <v>518</v>
       </c>
-      <c r="N51" s="2">
+      <c r="N51" s="1">
         <f t="shared" si="5"/>
         <v>210</v>
       </c>
@@ -4642,13 +4640,13 @@
       <c r="B52" t="s">
         <v>2</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C52">
         <v>784</v>
       </c>
-      <c r="D52" s="1">
+      <c r="D52">
         <v>544</v>
       </c>
-      <c r="E52" s="1">
+      <c r="E52">
         <v>205</v>
       </c>
       <c r="F52">
@@ -4660,24 +4658,24 @@
       <c r="H52">
         <v>205</v>
       </c>
-      <c r="I52" s="1">
+      <c r="I52">
         <v>784</v>
       </c>
-      <c r="J52" s="1">
+      <c r="J52">
         <v>544</v>
       </c>
-      <c r="K52" s="1">
+      <c r="K52">
         <v>205</v>
       </c>
-      <c r="L52" s="2">
+      <c r="L52" s="1">
         <f t="shared" si="3"/>
         <v>784</v>
       </c>
-      <c r="M52" s="2">
+      <c r="M52" s="1">
         <f t="shared" si="4"/>
         <v>544</v>
       </c>
-      <c r="N52" s="2">
+      <c r="N52" s="1">
         <f t="shared" si="5"/>
         <v>205</v>
       </c>
@@ -4725,13 +4723,13 @@
       <c r="B53" t="s">
         <v>3</v>
       </c>
-      <c r="C53" s="1">
+      <c r="C53">
         <v>256</v>
       </c>
-      <c r="D53" s="1">
+      <c r="D53">
         <v>551</v>
       </c>
-      <c r="E53" s="1">
+      <c r="E53">
         <v>239</v>
       </c>
       <c r="F53">
@@ -4743,24 +4741,24 @@
       <c r="H53">
         <v>242</v>
       </c>
-      <c r="I53" s="1">
+      <c r="I53">
         <v>256</v>
       </c>
-      <c r="J53" s="1">
+      <c r="J53">
         <v>550</v>
       </c>
-      <c r="K53" s="1">
+      <c r="K53">
         <v>241</v>
       </c>
-      <c r="L53" s="2">
+      <c r="L53" s="1">
         <f t="shared" si="3"/>
         <v>256</v>
       </c>
-      <c r="M53" s="2">
+      <c r="M53" s="1">
         <f t="shared" si="4"/>
         <v>551</v>
       </c>
-      <c r="N53" s="2">
+      <c r="N53" s="1">
         <f t="shared" si="5"/>
         <v>241</v>
       </c>
@@ -4808,13 +4806,13 @@
       <c r="B54" t="s">
         <v>4</v>
       </c>
-      <c r="C54" s="1">
+      <c r="C54">
         <v>263</v>
       </c>
-      <c r="D54" s="1">
+      <c r="D54">
         <v>567</v>
       </c>
-      <c r="E54" s="1">
+      <c r="E54">
         <v>233</v>
       </c>
       <c r="F54">
@@ -4826,24 +4824,24 @@
       <c r="H54">
         <v>231</v>
       </c>
-      <c r="I54" s="1">
+      <c r="I54">
         <v>264</v>
       </c>
-      <c r="J54" s="1">
+      <c r="J54">
         <v>574</v>
       </c>
-      <c r="K54" s="1">
+      <c r="K54">
         <v>233</v>
       </c>
-      <c r="L54" s="2">
+      <c r="L54" s="1">
         <f t="shared" si="3"/>
         <v>264</v>
       </c>
-      <c r="M54" s="2">
+      <c r="M54" s="1">
         <f t="shared" si="4"/>
         <v>574</v>
       </c>
-      <c r="N54" s="2">
+      <c r="N54" s="1">
         <f t="shared" si="5"/>
         <v>233</v>
       </c>
@@ -4891,13 +4889,13 @@
       <c r="B55" t="s">
         <v>1</v>
       </c>
-      <c r="C55" s="1">
+      <c r="C55">
         <v>782</v>
       </c>
-      <c r="D55" s="1">
+      <c r="D55">
         <v>491</v>
       </c>
-      <c r="E55" s="1">
+      <c r="E55">
         <v>250</v>
       </c>
       <c r="F55">
@@ -4909,24 +4907,24 @@
       <c r="H55">
         <v>250</v>
       </c>
-      <c r="I55" s="1">
+      <c r="I55">
         <v>784</v>
       </c>
-      <c r="J55" s="1">
+      <c r="J55">
         <v>490</v>
       </c>
-      <c r="K55" s="1">
+      <c r="K55">
         <v>251</v>
       </c>
-      <c r="L55" s="2">
+      <c r="L55" s="1">
         <f t="shared" si="3"/>
         <v>782</v>
       </c>
-      <c r="M55" s="2">
+      <c r="M55" s="1">
         <f t="shared" si="4"/>
         <v>491</v>
       </c>
-      <c r="N55" s="2">
+      <c r="N55" s="1">
         <f t="shared" si="5"/>
         <v>250</v>
       </c>
@@ -4974,13 +4972,13 @@
       <c r="B56" t="s">
         <v>2</v>
       </c>
-      <c r="C56" s="1">
+      <c r="C56">
         <v>774</v>
       </c>
-      <c r="D56" s="1">
+      <c r="D56">
         <v>516</v>
       </c>
-      <c r="E56" s="1">
+      <c r="E56">
         <v>214</v>
       </c>
       <c r="F56">
@@ -4992,26 +4990,25 @@
       <c r="H56">
         <v>214</v>
       </c>
-      <c r="I56" s="1">
+      <c r="I56">
         <v>773</v>
       </c>
-      <c r="J56" s="1">
+      <c r="J56">
         <v>516</v>
       </c>
-      <c r="K56" s="1">
+      <c r="K56">
         <v>243</v>
       </c>
-      <c r="L56" s="2">
+      <c r="L56" s="1">
         <f t="shared" si="3"/>
         <v>774</v>
       </c>
-      <c r="M56" s="2">
+      <c r="M56" s="1">
         <f t="shared" si="4"/>
         <v>516</v>
       </c>
-      <c r="N56" s="2">
-        <f t="shared" si="5"/>
-        <v>214</v>
+      <c r="N56" s="1">
+        <v>243</v>
       </c>
       <c r="O56">
         <f t="shared" si="6"/>
@@ -5023,7 +5020,7 @@
       </c>
       <c r="Q56">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="R56">
         <f t="shared" si="7"/>
@@ -5035,7 +5032,7 @@
       </c>
       <c r="T56">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="U56">
         <f t="shared" si="8"/>
@@ -5047,7 +5044,7 @@
       </c>
       <c r="W56">
         <f t="shared" si="14"/>
-        <v>-29</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.2">
@@ -5057,13 +5054,13 @@
       <c r="B57" t="s">
         <v>3</v>
       </c>
-      <c r="C57" s="1">
+      <c r="C57">
         <v>243</v>
       </c>
-      <c r="D57" s="1">
+      <c r="D57">
         <v>522</v>
       </c>
-      <c r="E57" s="1">
+      <c r="E57">
         <v>258</v>
       </c>
       <c r="F57">
@@ -5075,24 +5072,24 @@
       <c r="H57">
         <v>258</v>
       </c>
-      <c r="I57" s="1">
+      <c r="I57">
         <v>242</v>
       </c>
-      <c r="J57" s="1">
+      <c r="J57">
         <v>522</v>
       </c>
-      <c r="K57" s="1">
+      <c r="K57">
         <v>259</v>
       </c>
-      <c r="L57" s="2">
+      <c r="L57" s="1">
         <f t="shared" si="3"/>
         <v>243</v>
       </c>
-      <c r="M57" s="2">
+      <c r="M57" s="1">
         <f t="shared" si="4"/>
         <v>522</v>
       </c>
-      <c r="N57" s="2">
+      <c r="N57" s="1">
         <f t="shared" si="5"/>
         <v>258</v>
       </c>
@@ -5140,13 +5137,13 @@
       <c r="B58" t="s">
         <v>4</v>
       </c>
-      <c r="C58" s="1">
+      <c r="C58">
         <v>252</v>
       </c>
-      <c r="D58" s="1">
+      <c r="D58">
         <v>545</v>
       </c>
-      <c r="E58" s="1">
+      <c r="E58">
         <v>250</v>
       </c>
       <c r="F58">
@@ -5158,24 +5155,24 @@
       <c r="H58">
         <v>250</v>
       </c>
-      <c r="I58" s="1">
+      <c r="I58">
         <v>252</v>
       </c>
-      <c r="J58" s="1">
+      <c r="J58">
         <v>547</v>
       </c>
-      <c r="K58" s="1">
+      <c r="K58">
         <v>252</v>
       </c>
-      <c r="L58" s="2">
+      <c r="L58" s="1">
         <f t="shared" si="3"/>
         <v>252</v>
       </c>
-      <c r="M58" s="2">
+      <c r="M58" s="1">
         <f t="shared" si="4"/>
         <v>545</v>
       </c>
-      <c r="N58" s="2">
+      <c r="N58" s="1">
         <f t="shared" si="5"/>
         <v>250</v>
       </c>
@@ -5223,13 +5220,13 @@
       <c r="B59" t="s">
         <v>1</v>
       </c>
-      <c r="C59" s="1">
+      <c r="C59">
         <v>784</v>
       </c>
-      <c r="D59" s="1">
+      <c r="D59">
         <v>445</v>
       </c>
-      <c r="E59" s="1">
+      <c r="E59">
         <v>256</v>
       </c>
       <c r="F59">
@@ -5241,24 +5238,24 @@
       <c r="H59">
         <v>256</v>
       </c>
-      <c r="I59" s="1">
+      <c r="I59">
         <v>786</v>
       </c>
-      <c r="J59" s="1">
+      <c r="J59">
         <v>444</v>
       </c>
-      <c r="K59" s="1">
+      <c r="K59">
         <v>258</v>
       </c>
-      <c r="L59" s="2">
+      <c r="L59" s="1">
         <f t="shared" si="3"/>
         <v>784</v>
       </c>
-      <c r="M59" s="2">
+      <c r="M59" s="1">
         <f t="shared" si="4"/>
         <v>445</v>
       </c>
-      <c r="N59" s="2">
+      <c r="N59" s="1">
         <f t="shared" si="5"/>
         <v>256</v>
       </c>
@@ -5306,13 +5303,13 @@
       <c r="B60" t="s">
         <v>2</v>
       </c>
-      <c r="C60" s="1">
+      <c r="C60">
         <v>771</v>
       </c>
-      <c r="D60" s="1">
+      <c r="D60">
         <v>466</v>
       </c>
-      <c r="E60" s="1">
+      <c r="E60">
         <v>249</v>
       </c>
       <c r="F60">
@@ -5324,24 +5321,24 @@
       <c r="H60">
         <v>249</v>
       </c>
-      <c r="I60" s="1">
+      <c r="I60">
         <v>770</v>
       </c>
-      <c r="J60" s="1">
+      <c r="J60">
         <v>467</v>
       </c>
-      <c r="K60" s="1">
+      <c r="K60">
         <v>249</v>
       </c>
-      <c r="L60" s="2">
+      <c r="L60" s="1">
         <f t="shared" si="3"/>
         <v>771</v>
       </c>
-      <c r="M60" s="2">
+      <c r="M60" s="1">
         <f t="shared" si="4"/>
         <v>466</v>
       </c>
-      <c r="N60" s="2">
+      <c r="N60" s="1">
         <f t="shared" si="5"/>
         <v>249</v>
       </c>
@@ -5389,13 +5386,13 @@
       <c r="B61" t="s">
         <v>3</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C61">
         <v>233</v>
       </c>
-      <c r="D61" s="1">
+      <c r="D61">
         <v>414</v>
       </c>
-      <c r="E61" s="1">
+      <c r="E61">
         <v>255</v>
       </c>
       <c r="F61">
@@ -5407,24 +5404,24 @@
       <c r="H61">
         <v>255</v>
       </c>
-      <c r="I61" s="1">
+      <c r="I61">
         <v>234</v>
       </c>
-      <c r="J61" s="1">
+      <c r="J61">
         <v>415</v>
       </c>
-      <c r="K61" s="1">
+      <c r="K61">
         <v>254</v>
       </c>
-      <c r="L61" s="2">
+      <c r="L61" s="1">
         <f t="shared" si="3"/>
         <v>233</v>
       </c>
-      <c r="M61" s="2">
+      <c r="M61" s="1">
         <f t="shared" si="4"/>
         <v>414</v>
       </c>
-      <c r="N61" s="2">
+      <c r="N61" s="1">
         <f t="shared" si="5"/>
         <v>255</v>
       </c>
@@ -5472,13 +5469,13 @@
       <c r="B62" t="s">
         <v>4</v>
       </c>
-      <c r="C62" s="1">
+      <c r="C62">
         <v>243</v>
       </c>
-      <c r="D62" s="1">
+      <c r="D62">
         <v>441</v>
       </c>
-      <c r="E62" s="1">
+      <c r="E62">
         <v>245</v>
       </c>
       <c r="F62">
@@ -5490,24 +5487,24 @@
       <c r="H62">
         <v>245</v>
       </c>
-      <c r="I62" s="1">
+      <c r="I62">
         <v>245</v>
       </c>
-      <c r="J62" s="1">
+      <c r="J62">
         <v>441</v>
       </c>
-      <c r="K62" s="1">
+      <c r="K62">
         <v>246</v>
       </c>
-      <c r="L62" s="2">
+      <c r="L62" s="1">
         <f t="shared" si="3"/>
         <v>243</v>
       </c>
-      <c r="M62" s="2">
+      <c r="M62" s="1">
         <f t="shared" si="4"/>
         <v>441</v>
       </c>
-      <c r="N62" s="2">
+      <c r="N62" s="1">
         <f t="shared" si="5"/>
         <v>245</v>
       </c>
@@ -5555,13 +5552,13 @@
       <c r="B63" t="s">
         <v>1</v>
       </c>
-      <c r="C63" s="1">
+      <c r="C63">
         <v>745</v>
       </c>
-      <c r="D63" s="1">
+      <c r="D63">
         <v>492</v>
       </c>
-      <c r="E63" s="1">
+      <c r="E63">
         <v>198</v>
       </c>
       <c r="F63">
@@ -5573,24 +5570,24 @@
       <c r="H63">
         <v>198</v>
       </c>
-      <c r="I63" s="1">
+      <c r="I63">
         <v>744</v>
       </c>
-      <c r="J63" s="1">
+      <c r="J63">
         <v>492</v>
       </c>
-      <c r="K63" s="1">
+      <c r="K63">
         <v>198</v>
       </c>
-      <c r="L63" s="2">
+      <c r="L63" s="1">
         <f t="shared" si="3"/>
         <v>745</v>
       </c>
-      <c r="M63" s="2">
+      <c r="M63" s="1">
         <f t="shared" si="4"/>
         <v>492</v>
       </c>
-      <c r="N63" s="2">
+      <c r="N63" s="1">
         <f t="shared" si="5"/>
         <v>198</v>
       </c>
@@ -5638,13 +5635,13 @@
       <c r="B64" t="s">
         <v>2</v>
       </c>
-      <c r="C64" s="1">
+      <c r="C64">
         <v>731</v>
       </c>
-      <c r="D64" s="1">
+      <c r="D64">
         <v>517</v>
       </c>
-      <c r="E64" s="1">
+      <c r="E64">
         <v>189</v>
       </c>
       <c r="F64">
@@ -5656,24 +5653,24 @@
       <c r="H64">
         <v>189</v>
       </c>
-      <c r="I64" s="1">
+      <c r="I64">
         <v>730</v>
       </c>
-      <c r="J64" s="1">
+      <c r="J64">
         <v>515</v>
       </c>
-      <c r="K64" s="1">
+      <c r="K64">
         <v>190</v>
       </c>
-      <c r="L64" s="2">
+      <c r="L64" s="1">
         <f t="shared" si="3"/>
         <v>731</v>
       </c>
-      <c r="M64" s="2">
+      <c r="M64" s="1">
         <f t="shared" si="4"/>
         <v>517</v>
       </c>
-      <c r="N64" s="2">
+      <c r="N64" s="1">
         <f t="shared" si="5"/>
         <v>189</v>
       </c>
@@ -5721,13 +5718,13 @@
       <c r="B65" t="s">
         <v>3</v>
       </c>
-      <c r="C65" s="1">
+      <c r="C65">
         <v>258</v>
       </c>
-      <c r="D65" s="1">
+      <c r="D65">
         <v>462</v>
       </c>
-      <c r="E65" s="1">
+      <c r="E65">
         <v>221</v>
       </c>
       <c r="F65">
@@ -5739,24 +5736,24 @@
       <c r="H65">
         <v>221</v>
       </c>
-      <c r="I65" s="1">
+      <c r="I65">
         <v>256</v>
       </c>
-      <c r="J65" s="1">
+      <c r="J65">
         <v>461</v>
       </c>
-      <c r="K65" s="1">
+      <c r="K65">
         <v>223</v>
       </c>
-      <c r="L65" s="2">
+      <c r="L65" s="1">
         <f t="shared" si="3"/>
         <v>258</v>
       </c>
-      <c r="M65" s="2">
+      <c r="M65" s="1">
         <f t="shared" si="4"/>
         <v>462</v>
       </c>
-      <c r="N65" s="2">
+      <c r="N65" s="1">
         <f t="shared" si="5"/>
         <v>221</v>
       </c>
@@ -5804,13 +5801,13 @@
       <c r="B66" t="s">
         <v>4</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C66">
         <v>265</v>
       </c>
-      <c r="D66" s="1">
+      <c r="D66">
         <v>490</v>
       </c>
-      <c r="E66" s="1">
+      <c r="E66">
         <v>211</v>
       </c>
       <c r="F66">
@@ -5822,24 +5819,24 @@
       <c r="H66">
         <v>211</v>
       </c>
-      <c r="I66" s="1">
+      <c r="I66">
         <v>266</v>
       </c>
-      <c r="J66" s="1">
+      <c r="J66">
         <v>488</v>
       </c>
-      <c r="K66" s="1">
+      <c r="K66">
         <v>211</v>
       </c>
-      <c r="L66" s="2">
+      <c r="L66" s="1">
         <f t="shared" si="3"/>
         <v>265</v>
       </c>
-      <c r="M66" s="2">
+      <c r="M66" s="1">
         <f t="shared" si="4"/>
         <v>490</v>
       </c>
-      <c r="N66" s="2">
+      <c r="N66" s="1">
         <f t="shared" si="5"/>
         <v>211</v>
       </c>
@@ -5887,13 +5884,13 @@
       <c r="B67" t="s">
         <v>1</v>
       </c>
-      <c r="C67" s="1">
+      <c r="C67">
         <v>818</v>
       </c>
-      <c r="D67" s="1">
+      <c r="D67">
         <v>527</v>
       </c>
-      <c r="E67" s="1">
+      <c r="E67">
         <v>256</v>
       </c>
       <c r="F67">
@@ -5905,24 +5902,24 @@
       <c r="H67">
         <v>256</v>
       </c>
-      <c r="I67" s="1">
+      <c r="I67">
         <v>818</v>
       </c>
-      <c r="J67" s="1">
+      <c r="J67">
         <v>528</v>
       </c>
-      <c r="K67" s="1">
+      <c r="K67">
         <v>255</v>
       </c>
-      <c r="L67" s="2">
+      <c r="L67" s="1">
         <f t="shared" si="3"/>
         <v>818</v>
       </c>
-      <c r="M67" s="2">
+      <c r="M67" s="1">
         <f t="shared" si="4"/>
         <v>527</v>
       </c>
-      <c r="N67" s="2">
+      <c r="N67" s="1">
         <f t="shared" si="5"/>
         <v>256</v>
       </c>
@@ -5970,13 +5967,13 @@
       <c r="B68" t="s">
         <v>2</v>
       </c>
-      <c r="C68" s="1">
+      <c r="C68">
         <v>814</v>
       </c>
-      <c r="D68" s="1">
+      <c r="D68">
         <v>556</v>
       </c>
-      <c r="E68" s="1">
+      <c r="E68">
         <v>243</v>
       </c>
       <c r="F68">
@@ -5988,24 +5985,24 @@
       <c r="H68">
         <v>243</v>
       </c>
-      <c r="I68" s="1">
+      <c r="I68">
         <v>816</v>
       </c>
-      <c r="J68" s="1">
+      <c r="J68">
         <v>528</v>
       </c>
-      <c r="K68" s="1">
+      <c r="K68">
         <v>254</v>
       </c>
-      <c r="L68" s="2">
+      <c r="L68" s="1">
         <f t="shared" ref="L68:L82" si="15">MEDIAN(C68,F68,I68)</f>
         <v>814</v>
       </c>
-      <c r="M68" s="2">
+      <c r="M68" s="1">
         <f t="shared" ref="M68:M82" si="16">MEDIAN(D68,G68,J68)</f>
         <v>556</v>
       </c>
-      <c r="N68" s="2">
+      <c r="N68" s="1">
         <f t="shared" ref="N68:N82" si="17">MEDIAN(E68,H68,K68)</f>
         <v>243</v>
       </c>
@@ -6053,13 +6050,13 @@
       <c r="B69" t="s">
         <v>3</v>
       </c>
-      <c r="C69" s="1">
+      <c r="C69">
         <v>232</v>
       </c>
-      <c r="D69" s="1">
+      <c r="D69">
         <v>490</v>
       </c>
-      <c r="E69" s="1">
+      <c r="E69">
         <v>214</v>
       </c>
       <c r="F69">
@@ -6071,24 +6068,24 @@
       <c r="H69">
         <v>214</v>
       </c>
-      <c r="I69" s="1">
+      <c r="I69">
         <v>233</v>
       </c>
-      <c r="J69" s="1">
+      <c r="J69">
         <v>490</v>
       </c>
-      <c r="K69" s="1">
+      <c r="K69">
         <v>215</v>
       </c>
-      <c r="L69" s="2">
+      <c r="L69" s="1">
         <f t="shared" si="15"/>
         <v>232</v>
       </c>
-      <c r="M69" s="2">
+      <c r="M69" s="1">
         <f t="shared" si="16"/>
         <v>490</v>
       </c>
-      <c r="N69" s="2">
+      <c r="N69" s="1">
         <f t="shared" si="17"/>
         <v>214</v>
       </c>
@@ -6136,13 +6133,13 @@
       <c r="B70" t="s">
         <v>4</v>
       </c>
-      <c r="C70" s="1">
+      <c r="C70">
         <v>238</v>
       </c>
-      <c r="D70" s="1">
+      <c r="D70">
         <v>517</v>
       </c>
-      <c r="E70" s="1">
+      <c r="E70">
         <v>206</v>
       </c>
       <c r="F70">
@@ -6154,24 +6151,24 @@
       <c r="H70">
         <v>206</v>
       </c>
-      <c r="I70" s="1">
+      <c r="I70">
         <v>238</v>
       </c>
-      <c r="J70" s="1">
+      <c r="J70">
         <v>517</v>
       </c>
-      <c r="K70" s="1">
+      <c r="K70">
         <v>207</v>
       </c>
-      <c r="L70" s="2">
+      <c r="L70" s="1">
         <f t="shared" si="15"/>
         <v>238</v>
       </c>
-      <c r="M70" s="2">
+      <c r="M70" s="1">
         <f t="shared" si="16"/>
         <v>517</v>
       </c>
-      <c r="N70" s="2">
+      <c r="N70" s="1">
         <f t="shared" si="17"/>
         <v>206</v>
       </c>
@@ -6219,13 +6216,13 @@
       <c r="B71" t="s">
         <v>1</v>
       </c>
-      <c r="C71" s="1">
+      <c r="C71">
         <v>794</v>
       </c>
-      <c r="D71" s="1">
+      <c r="D71">
         <v>491</v>
       </c>
-      <c r="E71" s="1">
+      <c r="E71">
         <v>238</v>
       </c>
       <c r="F71">
@@ -6237,24 +6234,24 @@
       <c r="H71">
         <v>238</v>
       </c>
-      <c r="I71" s="1">
+      <c r="I71">
         <v>792</v>
       </c>
-      <c r="J71" s="1">
+      <c r="J71">
         <v>491</v>
       </c>
-      <c r="K71" s="1">
+      <c r="K71">
         <v>238</v>
       </c>
-      <c r="L71" s="2">
+      <c r="L71" s="1">
         <f t="shared" si="15"/>
         <v>794</v>
       </c>
-      <c r="M71" s="2">
+      <c r="M71" s="1">
         <f t="shared" si="16"/>
         <v>491</v>
       </c>
-      <c r="N71" s="2">
+      <c r="N71" s="1">
         <f t="shared" si="17"/>
         <v>238</v>
       </c>
@@ -6302,13 +6299,13 @@
       <c r="B72" t="s">
         <v>2</v>
       </c>
-      <c r="C72" s="1">
+      <c r="C72">
         <v>779</v>
       </c>
-      <c r="D72" s="1">
+      <c r="D72">
         <v>517</v>
       </c>
-      <c r="E72" s="1">
+      <c r="E72">
         <v>231</v>
       </c>
       <c r="F72">
@@ -6320,24 +6317,24 @@
       <c r="H72">
         <v>231</v>
       </c>
-      <c r="I72" s="1">
+      <c r="I72">
         <v>777</v>
       </c>
-      <c r="J72" s="1">
+      <c r="J72">
         <v>515</v>
       </c>
-      <c r="K72" s="1">
+      <c r="K72">
         <v>233</v>
       </c>
-      <c r="L72" s="2">
+      <c r="L72" s="1">
         <f t="shared" si="15"/>
         <v>779</v>
       </c>
-      <c r="M72" s="2">
+      <c r="M72" s="1">
         <f t="shared" si="16"/>
         <v>517</v>
       </c>
-      <c r="N72" s="2">
+      <c r="N72" s="1">
         <f t="shared" si="17"/>
         <v>231</v>
       </c>
@@ -6385,13 +6382,13 @@
       <c r="B73" t="s">
         <v>3</v>
       </c>
-      <c r="C73" s="1">
+      <c r="C73">
         <v>200</v>
       </c>
-      <c r="D73" s="1">
+      <c r="D73">
         <v>487</v>
       </c>
-      <c r="E73" s="1">
+      <c r="E73">
         <v>212</v>
       </c>
       <c r="F73">
@@ -6403,24 +6400,24 @@
       <c r="H73">
         <v>212</v>
       </c>
-      <c r="I73" s="1">
+      <c r="I73">
         <v>200</v>
       </c>
-      <c r="J73" s="1">
+      <c r="J73">
         <v>486</v>
       </c>
-      <c r="K73" s="1">
+      <c r="K73">
         <v>212</v>
       </c>
-      <c r="L73" s="2">
+      <c r="L73" s="1">
         <f t="shared" si="15"/>
         <v>200</v>
       </c>
-      <c r="M73" s="2">
+      <c r="M73" s="1">
         <f t="shared" si="16"/>
         <v>487</v>
       </c>
-      <c r="N73" s="2">
+      <c r="N73" s="1">
         <f t="shared" si="17"/>
         <v>212</v>
       </c>
@@ -6468,13 +6465,13 @@
       <c r="B74" t="s">
         <v>4</v>
       </c>
-      <c r="C74" s="1">
+      <c r="C74">
         <v>209</v>
       </c>
-      <c r="D74" s="1">
+      <c r="D74">
         <v>514</v>
       </c>
-      <c r="E74" s="1">
+      <c r="E74">
         <v>204</v>
       </c>
       <c r="F74">
@@ -6486,24 +6483,24 @@
       <c r="H74">
         <v>204</v>
       </c>
-      <c r="I74" s="1">
+      <c r="I74">
         <v>209</v>
       </c>
-      <c r="J74" s="1">
+      <c r="J74">
         <v>512</v>
       </c>
-      <c r="K74" s="1">
+      <c r="K74">
         <v>204</v>
       </c>
-      <c r="L74" s="2">
+      <c r="L74" s="1">
         <f t="shared" si="15"/>
         <v>209</v>
       </c>
-      <c r="M74" s="2">
+      <c r="M74" s="1">
         <f t="shared" si="16"/>
         <v>514</v>
       </c>
-      <c r="N74" s="2">
+      <c r="N74" s="1">
         <f t="shared" si="17"/>
         <v>204</v>
       </c>
@@ -6551,13 +6548,13 @@
       <c r="B75" t="s">
         <v>1</v>
       </c>
-      <c r="C75" s="1">
+      <c r="C75">
         <v>801</v>
       </c>
-      <c r="D75" s="1">
+      <c r="D75">
         <v>500</v>
       </c>
-      <c r="E75" s="1">
+      <c r="E75">
         <v>165</v>
       </c>
       <c r="F75">
@@ -6569,24 +6566,24 @@
       <c r="H75">
         <v>165</v>
       </c>
-      <c r="I75" s="1">
+      <c r="I75">
         <v>801</v>
       </c>
-      <c r="J75" s="1">
+      <c r="J75">
         <v>500</v>
       </c>
-      <c r="K75" s="1">
+      <c r="K75">
         <v>164</v>
       </c>
-      <c r="L75" s="2">
+      <c r="L75" s="1">
         <f t="shared" si="15"/>
         <v>801</v>
       </c>
-      <c r="M75" s="2">
+      <c r="M75" s="1">
         <f t="shared" si="16"/>
         <v>500</v>
       </c>
-      <c r="N75" s="2">
+      <c r="N75" s="1">
         <f t="shared" si="17"/>
         <v>165</v>
       </c>
@@ -6634,13 +6631,13 @@
       <c r="B76" t="s">
         <v>2</v>
       </c>
-      <c r="C76" s="1">
+      <c r="C76">
         <v>792</v>
       </c>
-      <c r="D76" s="1">
+      <c r="D76">
         <v>521</v>
       </c>
-      <c r="E76" s="1">
+      <c r="E76">
         <v>153</v>
       </c>
       <c r="F76">
@@ -6652,24 +6649,24 @@
       <c r="H76">
         <v>153</v>
       </c>
-      <c r="I76" s="1">
+      <c r="I76">
         <v>788</v>
       </c>
-      <c r="J76" s="1">
+      <c r="J76">
         <v>518</v>
       </c>
-      <c r="K76" s="1">
+      <c r="K76">
         <v>153</v>
       </c>
-      <c r="L76" s="2">
+      <c r="L76" s="1">
         <f t="shared" si="15"/>
         <v>792</v>
       </c>
-      <c r="M76" s="2">
+      <c r="M76" s="1">
         <f t="shared" si="16"/>
         <v>521</v>
       </c>
-      <c r="N76" s="2">
+      <c r="N76" s="1">
         <f t="shared" si="17"/>
         <v>153</v>
       </c>
@@ -6717,13 +6714,13 @@
       <c r="B77" t="s">
         <v>3</v>
       </c>
-      <c r="C77" s="1">
+      <c r="C77">
         <v>225</v>
       </c>
-      <c r="D77" s="1">
+      <c r="D77">
         <v>492</v>
       </c>
-      <c r="E77" s="1">
+      <c r="E77">
         <v>232</v>
       </c>
       <c r="F77">
@@ -6735,24 +6732,24 @@
       <c r="H77">
         <v>232</v>
       </c>
-      <c r="I77" s="1">
+      <c r="I77">
         <v>229</v>
       </c>
-      <c r="J77" s="1">
+      <c r="J77">
         <v>491</v>
       </c>
-      <c r="K77" s="1">
+      <c r="K77">
         <v>232</v>
       </c>
-      <c r="L77" s="2">
+      <c r="L77" s="1">
         <f t="shared" si="15"/>
         <v>225</v>
       </c>
-      <c r="M77" s="2">
+      <c r="M77" s="1">
         <f t="shared" si="16"/>
         <v>492</v>
       </c>
-      <c r="N77" s="2">
+      <c r="N77" s="1">
         <f t="shared" si="17"/>
         <v>232</v>
       </c>
@@ -6800,13 +6797,13 @@
       <c r="B78" t="s">
         <v>4</v>
       </c>
-      <c r="C78" s="1">
+      <c r="C78">
         <v>235</v>
       </c>
-      <c r="D78" s="1">
+      <c r="D78">
         <v>512</v>
       </c>
-      <c r="E78" s="1">
+      <c r="E78">
         <v>216</v>
       </c>
       <c r="F78">
@@ -6818,24 +6815,24 @@
       <c r="H78">
         <v>216</v>
       </c>
-      <c r="I78" s="1">
+      <c r="I78">
         <v>236</v>
       </c>
-      <c r="J78" s="1">
+      <c r="J78">
         <v>511</v>
       </c>
-      <c r="K78" s="1">
+      <c r="K78">
         <v>217</v>
       </c>
-      <c r="L78" s="2">
+      <c r="L78" s="1">
         <f t="shared" si="15"/>
         <v>235</v>
       </c>
-      <c r="M78" s="2">
+      <c r="M78" s="1">
         <f t="shared" si="16"/>
         <v>512</v>
       </c>
-      <c r="N78" s="2">
+      <c r="N78" s="1">
         <f t="shared" si="17"/>
         <v>216</v>
       </c>
@@ -6883,13 +6880,13 @@
       <c r="B79" t="s">
         <v>1</v>
       </c>
-      <c r="C79" s="1">
+      <c r="C79">
         <v>771</v>
       </c>
-      <c r="D79" s="1">
+      <c r="D79">
         <v>564</v>
       </c>
-      <c r="E79" s="1">
+      <c r="E79">
         <v>209</v>
       </c>
       <c r="F79">
@@ -6901,24 +6898,24 @@
       <c r="H79">
         <v>209</v>
       </c>
-      <c r="I79" s="1">
+      <c r="I79">
         <v>769</v>
       </c>
-      <c r="J79" s="1">
+      <c r="J79">
         <v>562</v>
       </c>
-      <c r="K79" s="1">
+      <c r="K79">
         <v>210</v>
       </c>
-      <c r="L79" s="2">
+      <c r="L79" s="1">
         <f t="shared" si="15"/>
         <v>771</v>
       </c>
-      <c r="M79" s="2">
+      <c r="M79" s="1">
         <f t="shared" si="16"/>
         <v>564</v>
       </c>
-      <c r="N79" s="2">
+      <c r="N79" s="1">
         <f t="shared" si="17"/>
         <v>209</v>
       </c>
@@ -6966,13 +6963,13 @@
       <c r="B80" t="s">
         <v>2</v>
       </c>
-      <c r="C80" s="1">
+      <c r="C80">
         <v>754</v>
       </c>
-      <c r="D80" s="1">
+      <c r="D80">
         <v>584</v>
       </c>
-      <c r="E80" s="1">
+      <c r="E80">
         <v>199</v>
       </c>
       <c r="F80">
@@ -6984,24 +6981,24 @@
       <c r="H80">
         <v>199</v>
       </c>
-      <c r="I80" s="1">
+      <c r="I80">
         <v>753</v>
       </c>
-      <c r="J80" s="1">
+      <c r="J80">
         <v>582</v>
       </c>
-      <c r="K80" s="1">
+      <c r="K80">
         <v>199</v>
       </c>
-      <c r="L80" s="2">
+      <c r="L80" s="1">
         <f t="shared" si="15"/>
         <v>754</v>
       </c>
-      <c r="M80" s="2">
+      <c r="M80" s="1">
         <f t="shared" si="16"/>
         <v>584</v>
       </c>
-      <c r="N80" s="2">
+      <c r="N80" s="1">
         <f t="shared" si="17"/>
         <v>199</v>
       </c>
@@ -7049,13 +7046,13 @@
       <c r="B81" t="s">
         <v>3</v>
       </c>
-      <c r="C81" s="1">
+      <c r="C81">
         <v>233</v>
       </c>
-      <c r="D81" s="1">
+      <c r="D81">
         <v>524</v>
       </c>
-      <c r="E81" s="1">
+      <c r="E81">
         <v>256</v>
       </c>
       <c r="F81">
@@ -7067,24 +7064,24 @@
       <c r="H81">
         <v>256</v>
       </c>
-      <c r="I81" s="1">
+      <c r="I81">
         <v>235</v>
       </c>
-      <c r="J81" s="1">
+      <c r="J81">
         <v>523</v>
       </c>
-      <c r="K81" s="1">
+      <c r="K81">
         <v>255</v>
       </c>
-      <c r="L81" s="2">
+      <c r="L81" s="1">
         <f t="shared" si="15"/>
         <v>233</v>
       </c>
-      <c r="M81" s="2">
+      <c r="M81" s="1">
         <f t="shared" si="16"/>
         <v>524</v>
       </c>
-      <c r="N81" s="2">
+      <c r="N81" s="1">
         <f t="shared" si="17"/>
         <v>256</v>
       </c>
@@ -7132,13 +7129,13 @@
       <c r="B82" t="s">
         <v>4</v>
       </c>
-      <c r="C82" s="1">
+      <c r="C82">
         <v>248</v>
       </c>
-      <c r="D82" s="1">
+      <c r="D82">
         <v>544</v>
       </c>
-      <c r="E82" s="1">
+      <c r="E82">
         <v>239</v>
       </c>
       <c r="F82">
@@ -7150,24 +7147,24 @@
       <c r="H82">
         <v>239</v>
       </c>
-      <c r="I82" s="1">
+      <c r="I82">
         <v>248</v>
       </c>
-      <c r="J82" s="1">
+      <c r="J82">
         <v>544</v>
       </c>
-      <c r="K82" s="1">
+      <c r="K82">
         <v>238</v>
       </c>
-      <c r="L82" s="2">
+      <c r="L82" s="1">
         <f t="shared" si="15"/>
         <v>248</v>
       </c>
-      <c r="M82" s="2">
+      <c r="M82" s="1">
         <f t="shared" si="16"/>
         <v>544</v>
       </c>
-      <c r="N82" s="2">
+      <c r="N82" s="1">
         <f t="shared" si="17"/>
         <v>239</v>
       </c>

</xml_diff>